<commit_message>
03/19/2025 Done TimeTickets Assigned, Add ka na lang Description and Subject dapat yung spaces is macancel ba and as well yung comma ata and quotes. Kaya mo yan :D
</commit_message>
<xml_diff>
--- a/HelpDeskVG/ReportFiles/TIMETAKENTOBEASSIGNED.xlsx
+++ b/HelpDeskVG/ReportFiles/TIMETAKENTOBEASSIGNED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOLID FIVE\source\repos\HelpDeskVG\HelpDeskVG\ReportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163268DE-9F05-4151-9F5B-349C00B5CC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1B400B-49A5-45A6-B1E7-C6A5C0F04681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="5850" windowWidth="22200" windowHeight="9810" xr2:uid="{D244A0FD-ECBF-44F2-AEEB-82E3871AC21A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D244A0FD-ECBF-44F2-AEEB-82E3871AC21A}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeTakenToBeAssignedTicket" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>TIME TAKEN TICKETS TO BE ASSIGNED</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>WITH THIRD PARTY?</t>
+  </si>
+  <si>
+    <t>FOR ASSIGNING CREATION DATE</t>
+  </si>
+  <si>
+    <t>ASSIGNMENT CONFIRMATION CREATION DATE</t>
   </si>
 </sst>
 </file>
@@ -122,10 +128,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,35 +465,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B47310-80CB-448B-BE31-C2C4947026FA}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="28.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1"/>
-    <col min="13" max="13" width="42.7109375" customWidth="1"/>
-    <col min="14" max="14" width="31" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="40.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" customWidth="1"/>
+    <col min="14" max="14" width="30.7109375" customWidth="1"/>
+    <col min="15" max="15" width="42.7109375" customWidth="1"/>
+    <col min="16" max="16" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -496,42 +504,47 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>